<commit_message>
Get daily reddit data: Tue Apr  9 08:08:11 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_14.xlsx
+++ b/data/2024_04_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C464"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2777 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1bzmdrx</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Spontaneous Ideas 🐉</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8ty4842retc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1bzlqdb</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Tried making marble nails for the first time for me and my sister! ೃ࿔*:･</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzlqdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1bzl84o</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Classic french press ons</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21psxyt5detc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1bzkua3</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Almond shape after long 💅</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzkua3</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1bzkn6e</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>issues with nail polish chipping super fast</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzkn6e</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1bzkhmq</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>I love this combination of colors.😍</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vuzo9pdv4etc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1bzkbv0</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Learning progress!</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzkbv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1bzk7jd</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>sagey 🤍</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jwt6nhtp1etc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1bzjya7</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>One of my very first sets that I did.</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzjya7</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1bzjy0w</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>My first time doing my nails, does the the thumb look odd?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzjy0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1bzjxqs</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>not sure if i love them or hate them 😭</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0040qmtydtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1bzjrep</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>My summer nails</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzjrep</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1bzj53e</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sometimes less is more </t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu8tdapvqdtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1bzj20h</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Cute 😍😍</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bk7g01g1qdtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1bzizyh</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>These ended up being my engagement nails!🤩💕</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzizyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1bzed64</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nail removal, what did I do wrong? </t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bzed64/press_on_nail_removal_what_did_i_do_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1bzieit</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Yellow nails</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmmb0iswjdtc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1bzidtd</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Finally have nails for the first time in forever! Can you tell I'm left handed?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blo12pjtjdtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1bzidd1</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>nails this week, matte sunny tan 😍</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9a7f0vojdtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1bz9tln</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>After 36 years on this earth, I’ve finally stopped biting my nails</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lu64otmkobtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1bz9mxj</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Can anyone tell me why my nails are like this :(</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19jr7ynanbtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1bz6rk5</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is a fair price for an acrylic overlay on short nails in only one color? </t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bz6rk5/what_is_a_fair_price_for_an_acrylic_overlay_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1bzgyso</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Orange/yellow monarch butterflies</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vb1lv597dtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1bz6h66</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>What are those actually for?</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bz6h66/what_are_those_actually_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1bzgdrp</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Prettiest pink 💖 #gelx</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7h8y7nd2dtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1bzf8nq</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Back to French for now</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxsfq14ssctc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1bzevuy</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail certification </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bzevuy/nail_certification/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1bzepcn</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Lilac Purple</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxb039bcoctc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1bzehq7</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>The set that made me quit</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sfy3ee0mmctc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1bzegvf</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>One of the few non-goth sets I got 💕</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fq5t80qfmctc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1bze1uk</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Help, how can I fix this?</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fm79l788jctc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1bzdvua</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Feeling like a mermaid</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzdvua</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1bzdhlc</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Tips for Making Press Ons?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bzdhlc/tips_for_making_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1bzde7u</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Do these look good?</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzde7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1bzddwl</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Celestial Eclipse Nails</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzddwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1bzcnpp</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>I just did my nails for the first time. Please give me some advice!</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w9a9r7zj8ctc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1bzcmrn</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>She’s amazing</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzcmrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1bzc6ei</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Gel manicure done at home 🩷</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54fr7y705ctc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1bzc640</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>They are beautiful, right? 🌹💋</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1m5lcby4ctc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1bzbl4f</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Russian manicure question</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bzbl4f/russian_manicure_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1bzbgn2</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Spring has sprung</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dy9s9euzbtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1bzbe8s</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>4 week retention 💚 regularly oiling my cuticles made such a difference in longevity</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzbe8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1bzbczl</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Ombré glitter set I did on myself this weekend</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzbczl</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1bzba2j</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>When it’s springtime but also it’s never not spooky season</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/km3bg6kkybtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1bzb0ok</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>17 year old nail artist here! Let me know what you like and what I can improve!</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzb0ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1bzaph6</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with the nails styling </t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5t5fk0mubtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1bzalh4</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In the nude </t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6womlattbtc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1bza64e</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Some color/pattern recommendations?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bza64e/some_colorpattern_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1bz9a78</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Spring nails 🌸 on a scale of 1-10 how much do these look like press ons? just wondering</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz9a78</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1bz8x8m</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Fav set this year 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz8x8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1bz81j5</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Decided on something springy and bright, super happy with it! </t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uu2sfvqhcbtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1bz7tsm</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>My nails for the eclipse</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmucxub3bbtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1bz7qhc</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>New spring nails I did on myself 😊</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz7qhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1bz76e1</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>simple 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lip4ab6q6btc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1bz6abj</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black french for a friend. </t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lr4c33og0btc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1bz616s</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Pearly Chrome</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz616s</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1bz2rdq</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Replacement for Dior abricot base?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bz2rdq/replacement_for_dior_abricot_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1bz3k75</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Glass nails</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz3k75</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1bz4rw5</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Which will damage my paper thin nails LEAST?</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bz4rw5/which_will_damage_my_paper_thin_nails_least/</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1bz4t24</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Hi, I'm a non-binary male who likes feminine nail art. Can anyone tell me what "in" this year for spring?</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bz4t24/hi_im_a_nonbinary_male_who_likes_feminine_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1bz5knv</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Lavender nails</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wqddpnobvatc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1bz50ww</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Is this cuticle oil any good?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3l9933ndratc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1bz4rs3</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Rose quartz + gold flakes = 💖</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz4rs3</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1bz47x4</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Just got my nails done what does Reddit think</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tke61tpqlatc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1bz44oy</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>My nail artist is 17 ✨</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz44oy</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1bz42zm</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>First time getting gel acrylic nails done .</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccxamh4tkatc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1bz3uix</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>new favorite set</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz3uix</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1bz36p2</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Nail n00b - need advice</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bz36p2/nail_n00b_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1bz33xy</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>New nails😍</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vup3dd3zdatc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1bz2vbd</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Bridal nails trial 🥰🎀</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz2vbd</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1bz2o9o</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz2o9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1bz2m2p</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Wife and I got matching pedicures for the eclipse</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9payb5xfaatc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1bz21db</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Some of my work that I did the past two weeks.</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz21db</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1bz1su8</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Top Coat for Gel- help!</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bz1su8/top_coat_for_gel_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1bz1nul</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Floral Nails</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz1nul</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1bz1lfa</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>nail set</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bz1lfa/nail_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1bz1lbp</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Trying to improve my gelx application. Any advice for a beginner? (ㅅ´ ˘ `)🌷</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75hwe57i3atc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1bz1gcl</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first nails </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0b93eoj2atc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1bz1fxt</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>My first jelly pedi</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zmtstsvg2atc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1bz1210</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Nude Pink</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2e4ev43oz9tc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1bz02ib</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Please help😩😩 ruined nails</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz02ib</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1bz0ofn</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Creeps after posting here</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6yf5lpq1x9tc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1byu0dx</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Sorry was doing other nail</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6tdu3tuka8tc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1bz04c6</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>eclipse nails🌕</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kasl3w63t9tc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1byzymi</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Help with Nail Salon Newbie</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1byzymi/help_with_nail_salon_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1byzyi5</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Alternative to Acrylics? </t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1byzyi5/alternative_to_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1byzrb5</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>First time getting my nails professionally done🍇</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2o3v5eniq9tc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1byzct9</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Starry nails!</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wwe3ku2in9tc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1byz2ft</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Short nails do not have to be boring. (Credit: Myself)</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1byz2ft</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1byy4x8</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Best topcoat for chrome</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1byy4x8/best_topcoat_for_chrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1byxzhk</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Pink has me in a chokehold</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xp39333d9tc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1byxyph</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Stars and nude base</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nparvuuwc9tc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1byxma6</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Purple on black aesthetic</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1byxma6/purple_on_black_aesthetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1byx6xc</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Next interesting style, how it looks like?</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4pb5mzfe69tc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1byvwgl</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>The two sets of nails I've had the past two months 😁 the frogs are my favourite 😍</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1byvwgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1byv73m</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Ombré chrome obsessed!</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1byv73m</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1byua3l</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>From summery to simmer-y?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1byua3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1bysvrf</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Nail art that isn’t pretty.</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bysvrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1bysp4q</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Feeling Lit ✨️</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aovf3ghqu7tc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1bzjqpc</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzjqpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1bzjewy</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>She Was Enough by BKL! I'm obsessssssed</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzjewy</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1bzj4xv</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Unintentionally Easter? 🐣</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dw80z7fuqdtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1bzidxi</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Shrinking</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bzidxi/dazzle_dry_shrinking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1bzi5wh</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Nail polish outlasted the nail at work</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzi5wh</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1bzhxra</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>In love with this polish from CVS 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzhxra</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1bzhf0l</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>ILNP Eclipse mani during eclipse totality</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzhf0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1bzgtg0</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Wife did an eclipse-themed paint job and I love it🌌</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8di1fxy5dtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1bzg7v2</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Mooncat Highway Glow &amp; Portrait of an Introvert</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzouy22y0dtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1bzf9cj</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>I couldn’t decide on a color so I did them all! Skittles of my new polishes from Cirque Colors and some other polishes I’ve been wanting to wear</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzf9cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1bzf7nw</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Death Valley Nails' new "Eating Heads: a Praying Mantis Love Story"</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ndsl8h1fsctc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1bzf754</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>I can't stop staring</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zsvhxncesctc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1bzcoz5</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Poisonberry 🫐</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzcoz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1bzbmxq</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Sooo... we're all wearing ILNP Eclipse today, right?</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzbmxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1bzbjv3</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Cute nails for this week. Note for next time, don't use golf for outlines! Hehe</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzbjv3</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1bzbfmc</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Joining the ILNP Eclipse club! 🌒</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzbfmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1bzbc3k</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Birthday Eclipse Comet nails</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzbc3k</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1bzb7vc</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>SpongeBob Nailtopia Collection</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upi0rwb5ybtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1bz9nop</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Like a party on my nails 🤩</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7uk08egnbtc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1bz9jnj</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Chibi Chibi is a Barbie shimmer wet dream</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz9jnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1bz99ik</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>I forgot about the eclipse…here’s some bleeding roses instead!</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz99ik</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1bz92or</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>My Eclipse Day nails…that didn’t quite pan out.</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz92or</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1bz8ass</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>show me your eclipse nails 🤗</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz8ass</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1bz8588</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Honestly really pissed that there was no notice before purchase but pls help with the 110 specifically</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz8588</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1bz83ze</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>I didn’t have Eclipse so I decided to use Haunted Melody 🎶</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kt97e72xcbtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1bz8126</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Another blurple crelly</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ec87alsecbtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1bz6qkp</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>What are those actually for?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bz6qkp/what_are_those_actually_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1bz7qjw</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Brighter take on eclipse nails</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz7qjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1bz6rkp</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Who else is wearing Eclipse during the eclipse?</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz6rkp</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1bz60z4</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Polar Light Show</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz60z4</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1bz57pm</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails in the eclipse, rn </t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9lot6lspsatc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1bz4k0h</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Happy Eclipse Day!</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz4k0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1bz4eux</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>My eclipse mani!</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz4eux</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1bz3w6y</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Mooncat - Cheshire Cat 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz3w6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1bz2x40</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Is it too late to post eclipse nails?</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz2x40</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1bz1d1h</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>An option for mermaids</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz1d1h</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1bz157f</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Saw everyone wearing ILNP Eclipse for eclipse day, so I had to do it immediately, but with an added twist!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz157f</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1bz0t0s</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Celebrating the Eclipse mani</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz0t0s</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1bz0jf6</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>🌑🌒🌓🌔🌕</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz0jf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1byzoxh</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>My Eclipse Mani</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1byzoxh</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1byzgk7</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Rarest of them All</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1byzgk7</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1byz1jt</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Eclipse nails but not using ILNP Eclipse</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1byz1jt</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1byywaw</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Twilight’s eclipse on ILNP’s eclipse during an eclipse…groundbreaking</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yix4yj53k9tc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1byyq1a</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Wearing ILNP’s Eclipse on an Eclipse…groundbreaking</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1byyq1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1byyeqh</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Jazzy nudes</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11kfjccfg9tc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1byy6rs</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>The shift of ILNP Cygnus loop is just incredible! Cat tax included in all pictures ❤️</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1byy6rs</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1byxyk7</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>More abstract eclipse nails!</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08siihpvc9tc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1byxlbt</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>I hate this polish!!!</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1byxlbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1byxk27</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Solar Flare, Solar Unicorn Skin, Eclipse 🌙 ☀️</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1byxk27</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1bywst4</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>ORLY Metamorphosis</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bywst4</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1byu2nm</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1byu2nm/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1bythal</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Addicted to nudes</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bythal</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1bysmre</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Glowing 🌊</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bysmre</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1bzkhw0</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Butterfly vibes 🦋🩷💜</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acx7vhey4etc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1bzhuy2</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frenchies with Starbursts </t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0eqtk0tzedtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1bzf51y</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>🌈 Lisa Frank Inspired 🌈</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gq94tmyxrctc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1bz57kd</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Eclipse Nails</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz57kd</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1bz4u3m</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Rose quartz + gold flakes 💖</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz4u3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1bz2dfj</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>💟</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bz2dfj</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1bz1zli</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Solar Eclipse-Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhsxvaoa5atc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1bywpgr</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Just another spring set ✨ Loving the flower themes rn 🌸</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bywpgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1byw6lu</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>What gel polish would I need for the base color?</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/abc2jjhjx8tc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1bytjrh</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>My first attempt at Encapsulated Polygel Nails. Did I nail it ??</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xgxxjtm558tc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1bysimj</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Depression is real</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bysimj</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Apr 10 08:09:07 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_14.xlsx
+++ b/data/2024_04_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C464"/>
+  <dimension ref="A1:C574"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8321,6 +8321,1876 @@
         </is>
       </c>
     </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1c0ga3e</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Anyone know what could this be?</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ok9ry7qxzltc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1c0g6fh</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>I like them shorter, they seem more presentable and comfortable for my routine 💋 I love them 🙈</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q08mntwnyltc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1c0fmg0</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>I think I like this set</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/od8evcvprltc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1c0f8w1</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Chrome nails peeling</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1zmp5j4nltc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1c0es1o</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Any recommendations for a shiny top coat that doesn’t go dull the next day or by touch?</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6pa57fnhltc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1c01wdg</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Help me understand and describe what I need done to my nails</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c01wdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1c0e2u8</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Does anyone have a dupe for (discontinued) OPI Elegance ?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c0e2u8/does_anyone_have_a_dupe_for_discontinued_opi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1c0dwqe</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Simple French</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tux2ud808ltc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1c0ctwi</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Magnetic Purple Cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0ctwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1c09zv6</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Vacation Nails!!</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c09zv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1c07zj3</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Life in color neon</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8p19ik0aqjtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1c07v7k</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>What you guys think</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kixxunh9pjtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1c07hou</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>What was your epic nail fail? I’ll go first🤣🫗</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c07hou</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1c07h7y</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Feeling fancy now 🥰🥰</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c07h7y</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1c079i4</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>What do y’all think about these?</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rz4vd5sckjtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1c075td</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>mermaid blue</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49chpt8mjjtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1c06ywp</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>I tried</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hiae19d1ijtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1c06y7x</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Blue nails for April</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c06y7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1c06g4b</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Transparent nude and first time trying almond shaped nails</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c06g4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1c06e00</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Salon xtend</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c06e00/salon_xtend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1c065lu</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>something about long nails I just can’t get enough of.🖤</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c065lu</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1c0651v</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Cherry Coquette Nails</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0651v</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1c05v9c</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Look at Those "pinks"..it's the perfect combination, isn't it?🩷</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5nwncc9r9jtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1c05bnh</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Spring Nails 🌼</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c05bnh</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1c054fy</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>set of falsies i just made !</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c054fy</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1c04osf</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>How badly have I messed up my nails?</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z77945k31jtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1c04lp4</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>My nail growth journey</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/smhxedkj0jtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1c02ron</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>:)</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/allpxluenitc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1c02kt9</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>What can I add?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zchkj6d0mitc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1c02bbc</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Gel nails🌷</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axbfbue1kitc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1c01r0v</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Did my own nails for the very first time today! Found out i really can't draw stars. How did i do?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70o6nptyfitc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1c00ntz</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Red love 😘❤️🍎</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8f19ry08itc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1bzzixp</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Ordered Aurora Queen's "Flowering" glitter set and one of the bottles turned out empty. -Has this ever happened to you?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzzixp</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1bzz3wf</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>My new nails 💅</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bjnjz1swhtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1bzyb4q</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Simple palate cleanser ✨</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzyb4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1bzy8il</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>had to make it extra special for my 20th 🥳</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nhqesr2kqhtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1bzxq4p</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>After battling brittle nails from repetitive gel applications, my nails are strong again!</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k63js2sqmhtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1bzxax5</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>What do we think? Too much?</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sio3upoljhtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1bzv8pw</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Best shape??</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzv8pw</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1bzuzub</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Marble and matte 💜</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlebi0ik2htc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1bzusiv</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone know why the whites of my nails are so large? Can I fix this somehow? </t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdfkwyr51htc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1bzqvpe</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Which nail shape is good for me?</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzqvpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1bztwlh</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>New Gel-x set</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bztwlh</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1bzt4uu</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t xml:space="preserve">dollar tree glue ons </t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bc88ygkoogtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1bzt41v</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Got my nails done today.:)</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vojpljzhogtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1bzt0rc</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome, room for improvement but my second time using builder gel, first time using chrome powder </t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xq8odqzrngtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1bzswh5</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Shorties are cute too?</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzswh5</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1bzspl8</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>How can I speed up the growth of my nails? Im already using strenghtener and 1 nail just wont grow. Is there any home remedies i can try?</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bzspl8/how_can_i_speed_up_the_growth_of_my_nails_im/</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1bzsmap</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>First time having nail extensions and I feel like a princess!</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pgh2bjmkgtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1bzsa79</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>I think this set is my new personal favourite 😻</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzsa79</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1bzr7p8</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Freehand black goldfish ✨ any suggestions?</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s5tyvszz8gtc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1bzqt8t</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>First attempts at semi-permanent</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzqt8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1bzqq6d</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Color combo ⭐🙈💋</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pd9opx1p4gtc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1bzof1t</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Gel polish help!</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1bzof1t/gel_polish_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1bzocqd</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Tried poly gel for the first time !!</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clfds4vhgftc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1bznkqd</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>spring nails 🪷🌱🌸🌵🩰🌴🌸</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bznkqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1bzn8su</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Should I stick with shorter nails?</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzn8su</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1c0g4ex</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Sheer pink glitters/shimmers?</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0g4ex</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1c0fqfa</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Can I put a new layer of polish over topcoat in order to cover up nail outgrowth?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c0fqfa/can_i_put_a_new_layer_of_polish_over_topcoat_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1c0et1y</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Favorite Essie shades?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c0et1y/favorite_essie_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1c0du25</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Broke my ankle, but at least my pedi looks good!</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xp5tqn767ltc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1c0cn63</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Fairy dust dupe help</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0cn63</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1c0cgm4</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Any nail polish dupe color to Dashing Diva Rosy Cheeks?</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6a8pzxe4tktc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1c0ccwn</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer- Amid the insects’ lulling serenade</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m7qolht7sktc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1c0b2l7</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>In love with this icy blue!</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0b2l7</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1c0acl3</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>ILNP Salem 🧙🏻‍♀️✨</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9268xle5aktc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1c09sf6</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You ever have a day where you feel grumpy and then you throw on a different polish and your whole attitude turns around? </t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/btfnvlod5ktc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1c08f4j</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>love indie polish! (death valley nails)</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhwcnt8utjtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1c08bu5</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Anyone Else Have A Sentimental Bottle?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c08bu5</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1c07yqj</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite set so far! Holo Taco-Frost Light! </t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h3tr4um2qjtc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1c07ver</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Pahlish - Long Story Short</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fjuueyt9pjtc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1c07u67</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Swamp Gloss “Thoughts and Prayers, Frodo”</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c07u67</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1c06ud8</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Atropa Belladonna 🍃</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c06ud8</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1c065de</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Florist here, My nails are horrible. help.</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qdeqyhtbjtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1c062hv</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>What's your favourite gold polish?</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c062hv/whats_your_favourite_gold_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1c05ma5</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Holo taco Circut Breaker</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c05ma5</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1c058j2</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Skittle mani of the polishes that started it all 🥹🫶🏻</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c058j2</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1c04txt</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>The Perfect Pearl 🦪</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c04txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1c03xp2</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>some bright blue for spring start 🔷</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c03xp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1c0252r</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>I think I may have finally found my perfect nude (combo)!</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/41dnd8qpiitc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1c01haq</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>This polish gets the pug snort of approval</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j8sgbtj2eitc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1c01coe</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Do peel off base coats cause damage? How long does a mani last?  Brand recommendations?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c01coe/do_peel_off_base_coats_cause_damage_how_long_does/</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1c013p2</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Holo Taco- Play Rosé</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdrr5chcbitc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1bzzq8h</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Orange Creme</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/hA4yTmX</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1bzzpy5</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Spring has sprung</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzzpy5</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1bzzi1i</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>I Want My MTV</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c3qfh7sjzhtc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1bzz2u8</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Feeling some mellow spring valley vibes featuring some dill!</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/fxBX6wk</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1bzyxdd</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Out on Your Street</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzyxdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1bzwx21</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Magnetic polish</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fnrl1etrghtc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1bzwu3r</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Eclipse nails in totality</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzwu3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1bzwphb</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kitten manicure </t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axqwayq5fhtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1bzums6</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>⚡️💙Blue Ranger💙⚡️</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzums6</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1bzm7vt</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Is it possible for damaged nails to grow up in shape?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bzm7vt/is_it_possible_for_damaged_nails_to_grow_up_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1bzu0o6</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>I think i need to chill with nail polish...</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1bzu0o6/i_think_i_need_to_chill_with_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1bzt87e</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Lipgloss nails ✨</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzt87e</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1bzsbhj</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>It’s starting to feel like Spring</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzsbhj</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1bzs1cj</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Poppy Jelly</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzs1cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1bzrczp</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Manifesting cherry season with this mani 🍒</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzrczp</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1bzq3bn</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Expressie Toppers?</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzq3bn</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1c0b2ed</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Freestyle birthday nails 🥳💜</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0b2ed</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1c04qju</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Spring Nails 🌺</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c04qju</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1c03efa</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Did my sister's nails</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hmubytyritc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1c02cwj</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Fiesta / Spring Nails</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c02cwj</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1c01p77</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Spring Lemon Nails! </t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iu4vnlamfitc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1c00kek</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>My Silver Chrome Set IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnao47ob7itc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1bzyj6b</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>In my dinosaur era 🦕 💅🏻</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzyj6b</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1bzxly3</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Quite proud of this cherry blossom set I did a few days ago! Just sad I didn't get any better pics of it, these pics really doesn't do the colours justice.</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzxly3</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1bzxj2d</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Steam punk design</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzxj2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1bzs9g7</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>I think this set is my new personal favourite 😻</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1bzs9g7</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1bzplz2</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Easter bunny nails</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ive5xbo6uftc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Apr 11 08:08:08 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_14.xlsx
+++ b/data/2024_04_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C574"/>
+  <dimension ref="A1:C734"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10191,6 +10191,2726 @@
         </is>
       </c>
     </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1c19gjx</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Tips for how to apply press ons?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c19gjx/tips_for_how_to_apply_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1c19e3l</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Constantly having problems with nail glue</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c19e3l/constantly_having_problems_with_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1c191oo</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>is this pink a good color on me?(if not, any recommendations?)</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c191oo</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1c18ent</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Redid my nails to be ready for my birthday 🎂</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c18ent</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1c18cs9</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>3rd time doing my own set</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qjehl6cqstc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1c183nh</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New to at home manicures </t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c183nh/new_to_at_home_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1c17ofo</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Made two re-useable sets today. A "psychedelic", and "princess" set.</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4lhsa1zwistc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1c17g79</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Hi</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c17g79</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1c17g22</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>are my nail beds too short/small for press ons?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/io3jmncdgstc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1c16khh</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Neon pink + chrome = 🧑🏻‍🍳💋</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i9ihn0647stc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1c15a6c</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Nailtiques Formula 2 causing burning sensation!</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c15a6c/nailtiques_formula_2_causing_burning_sensation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1c157bb</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Unintentionally matched my nails to my wrist sleeve today.</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08dk83altrtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1c151ih</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Update on my nail post from a couple days ago!</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c151ih</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1c15124</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>new set today 😁</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o26tornurrtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1c14nvc</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Sistaco Nails - Help! Express Remover is BAD.</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c14nvc/sistaco_nails_help_express_remover_is_bad/</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1c14t61</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>My girl did it again 🔥✨</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c14t61</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1c12f6v</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>What is the best option for temporary fake nails for an event, that isn’t press ons? (But you want to take off the next day?)</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c12f6v/what_is_the_best_option_for_temporary_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1c10j8z</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Dents and discoloration in Luminary nails</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zeh8oxgfpqtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1c10b79</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>This was not at ALL what I asked for, but they’re starting to grow on me 😌</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uuo2mkflnqtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1c0yz4p</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Newbie Questions</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c0yz4p/newbie_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1c0yxhz</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>what nails should i get done for my prom</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fm5b7iqucqtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1c0x3up</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Can't get these press ons off. Ruining nails in the process.</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c0x3up/cant_get_these_press_ons_off_ruining_nails_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1c14lb6</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Love this color</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4h1jxd2rnrtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1c147ox</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Off Hand Work</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c147ox</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1c143ru</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>🙂</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6m3y97ejrtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1c13tiv</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Aurora borealis ✨ how many colors do you see?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8yypoqvgrtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1c13i8d</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>White Coffin Nails🤍</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zh8wz2x6ertc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1c13f0o</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Working on getting my natural nails healthy again, glad I can still paint them :)</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c13f0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1c1160p</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Cherry red nail set</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c1160p/cherry_red_nail_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1c0tn4f</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Eclipse Nails: What I asked for vs what I got. Inspo credit to ChickenScratchNails on Etsy</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0tn4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1c10bku</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>my nails tech ATE with this set @thenaildrip on IG</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c10bku</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1c0zd6h</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Getting my nails done tomorrow for the first time since 2022! Going for Builder (IAB), which I’ve never had before. What to expect? </t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c0zd6h/getting_my_nails_done_tomorrow_for_the_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1c0z758</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Latest set 😍</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0z758</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1c0z5kx</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Went for a full set today! 💜💚👽</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0z5kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1c0ymz4</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>A husband on a mission - We didn't really do Easter nails. These remind me of something my daughter would request.</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0ymz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1c0xtmb</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>I know it's a week late, but.. do you like my Easter nails? (ㅅ´ ˘ `)🌷</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0xtmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1c0xsl0</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>I found a nail tech!</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8m9bixh4qtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1c0xsa4</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Got muh nails did! 😈😈😈</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0xsa4</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1c0xbsl</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Pink Wednesday 🥰</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c0xbsl/pink_wednesday/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1c0xaqx</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>white/pearl chrome</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0xaqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1c0wwg3</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Beginner nail tech here! First time doing croc print and I’m in love!</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knv1vac0yptc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1c0wfcr</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Tried something different🩵</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khis8ycjuptc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1c0w6f9</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Smiling friends nail art 🤌🏼✨</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0w6f9</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1c0w1da</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Plum 💟</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gndipvolrptc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1c0vz41</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>black hearts 🖤</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0vz41</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1c0vpb8</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Do Gel X extensions usually have this much gel underneath?</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0vpb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1c0vlfh</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Love how the press ons blend with the natural nails</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0vlfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1c0uetq</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Nail Artist is Amazing! </t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yq9an5o0gptc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1c0u9gl</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Pink marble 💗</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vij2cpixeptc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1c0u82h</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>hi all, i’m 19 and did nail tech school last summer. here’s some sets i’ve done!</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0u82h</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1c0u45g</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Update! Cruise Nails</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0u45g</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1c0trnu</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>coquette nails</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0trnu</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1c0tjny</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Alternative to Gel Builder? I used to always get shellac but my nails always broke, so my nail tech recommended gel builder. Unfortunately I don't like how they look or how chunky they are. I really want to keep getting my nails done, I'm wondering if there's a strong alternative that's not chunky</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3asaeh3r9ptc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1c0teqm</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>DIY spring nails</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0teqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1c0t32h</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>A nail shaming group hated these. Are they really that bad?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrses76e6ptc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1c0sp7s</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>The Mold and the Beautiful</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0sp7s</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1c0sasf</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Can i fix this at home with a file?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0sasf</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1c0pu9u</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>First set of acrylics</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0h4cjecpiotc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1c0ptjs</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Does anyone know what OPI color this is?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5486gu8kiotc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1c0j2vh</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Van Cleef inspo</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0j2vh</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1c0in9d</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice for irritated cuticles? </t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c0in9d/advice_for_irritated_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1c0gl6v</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>why do my nails grow like this?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0gl6v</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1c0s5oq</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Loving these mix and match nails</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0s5oq</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1c0rws0</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>what the difference between this two set of tips? Which ones can be applied with glue?</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0rws0</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1c0rt5x</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Bee nails🐝</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2au0nqw6xotc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1c0r60q</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Natural nails ❤️❤️❤️</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0r60q</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1c0prgb</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Love for classics 🖤</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1x3lb5m5iotc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1c0pii1</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Spring nails acrylic  without tips</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/temcijx9gotc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1c0pfo9</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>♥️Second attempt at french tips♥️</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0pfo9</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1c0pee5</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>♥️ Red</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0pee5</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1c0p4ou</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Feeling purple 💟</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/el95cqpedotc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1c0ok4c</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Light blue Ombre on natural nails 💙</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vo6xsb349otc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1c0n9pf</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Mia at Uptown Nails in VA is the best! Soft pink chrome nails! Obsessed!</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ssp5w0pezntc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1c0mcy3</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>lavender haze 💟</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajnwc4z6sntc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1c0l7j1</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Questions (inspo from Instagram account gelpolish_bar)</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9sgdhz2tintc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1c0la2p</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Is there a base coat that works with polygel and hard gel?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c0la2p/is_there_a_base_coat_that_works_with_polygel_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1c0ln2x</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Trying darker shades, and I think it's growing on me!</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0pmo3kpgmntc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1c0leog</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>How far I’ve come with an amazing tech</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0leog</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1c0l7xc</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Nail Drill Recs?</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c0l7xc/nail_drill_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1c0k9vm</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>I fell in love with This pearly color!🤍</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0k9vm</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1c0jh7k</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Graffiti set -part 4</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0jh7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1c0iotj</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Iridiscent blue french tips</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0iotj</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1c0hmem</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Water nails 🏝️</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcx3lf5lhmtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1c0gyey</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Nails for a NYC trip</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/46gsc0xx8mtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1c0guey</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Ohh, airbrush 💔💔💔</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0guey</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1c0guch</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Nail polish not applying properly to two specific fingers?</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c0guch/nail_polish_not_applying_properly_to_two_specific/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1c17pck</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>ZERO nail polish</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57fitvt5jstc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1c15gkg</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>ISO: Vampy jellies</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eko23dw4wrtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1c12exx</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Toxin free drugstore top &amp; base coats?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c12exx/toxin_free_drugstore_top_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1c140pm</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>OPI polish changing color in the sun???</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c140pm/opi_polish_changing_color_in_the_sun/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1c132yb</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>BKL HOFAS 🧲</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c132yb</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1c12i4i</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Clean look with gems</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c12i4i</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1c1271b</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Trying solar polish!</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1271b</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1c126rv</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Tried to study but couldn't stop looking at my nails. I'm so proud of them!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c126rv</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1c11n1i</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Nail Shape Changing?</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c11n1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1c11k1o</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>A Juicy Jelly and Some Strawberries</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c11k1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1c11hfu</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Past couple of manis</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c11hfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1c116hy</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>This shade is so delicate 🎀</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c116hy</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1c111s5</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>🌟 she glow 🌟</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1cbqjrgtqtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1c10l8q</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Just found RedditLaqueristas, and I'm in heaven! Most recent mani for tax!</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c10l8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1c0zx56</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Spreading around some Fairy Dust 🧚</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jhjfqygkqtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1c0z487</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>You always be my sister</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eapbxm0beqtc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1c0yxu9</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>First EDM and I’m IMPRESSED</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0yxu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1c0y0rn</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>French Skittle! 🩷</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0y0rn</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1c0xx75</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How many Mooncats does a Helmer hold? </t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ww95rimf5qtc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1c0xpq0</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Alchemy - Stiff as a Board</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0xpq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1c0wyod</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does this happen to anyone else? </t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c0wyod/does_this_happen_to_anyone_else/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1c0wrtg</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>What’s going on with my nail?</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zyqshl2xptc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1c0whyf</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Rainbow time!!!</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0whyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1c0wfja</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>“Sometimes there’s so much beauty in the world, I feel like I can’t take it.”</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0wfja</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1c0uryc</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>LynBDesigns Embrace the Mess</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0uryc</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1c0uj0z</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Gradients?</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c0uj0z/gradients/</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1c0uip8</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Devastated</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0uip8</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1c0tqvu</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Didn’t love the way I applied the milky color on top so experimented a bit</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0tqvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1c0tpol</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Just a Notion 🔮- Emily De Molly</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/14jgrzkvaptc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1c0tnhc</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Do we like these? Or should I take them off?</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wydm540japtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1c0timx</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Has anyone tried the Essie jelly polishes?</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qawxfy5k9ptc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1c0sxec</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Essie Cactus Jelly</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0sxec</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1c0suj6</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Help with nail color for Indian bride!</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0suj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1c0ssw6</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Obsessed with jellies 🪼</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8f04ryd4ptc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1c0so19</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Spring Aesthetic Cat Eye Gel with Chrome Accent</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0so19</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1c0sf49</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Cut down blue</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c0sf49/cut_down_blue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1c0qew0</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Greens and Blues like the Sea</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0qew0</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1c0pmox</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Birthday month nails</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0pmox</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1c0p7gy</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>trickster fox</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0p7gy</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1c0o5hg</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Broke a nail and had to go back to short! But I feel like shorties look good in green 💚🥝🍐</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0o5hg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1c0o3bi</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Cruelty Free Dupe for OPI Kyoto Pearl</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wkawy7sn5otc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1c0nseb</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Another of my "Shopping from my stash" manis</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3facn3ec3otc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1c0n9nk</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for a perfect "90's baby blue" shade. </t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c0n9nk/looking_for_a_perfect_90s_baby_blue_shade/</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1c0n3m0</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Some rose gold line art - actually quite pleased with how this turned out.</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkhy0662yntc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1c0n0oh</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>when your polish matches your fidget toy &gt;&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yl4qavgexntc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1c0myz5</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>The Crab 🦀</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0myz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1c0mv7e</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>These reminded me of a tropical sunset 🍹</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pu6zrp6wntc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1c0moj1</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>The Curse Of Calypso</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0moj1</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1c0memk</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>When you simply can’t capture the polish’s beauty</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0memk</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1c0ltji</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>What does she put on top of the marble layer?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c0ltji/what_does_she_put_on_top_of_the_marble_layer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1c0lrr7</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Please tell me I'm not the only one who does this 🤦🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0lrr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1c0l5v4</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Busy bees among the flowers 🐝</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u2lh9n9eintc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1c0inuy</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Spring Sprinkles</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0bbxi2ztmtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1c0hepk</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>You're finally awake</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0hepk</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1c0ha0m</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Recovery suggestions</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c0ha0m/recovery_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1c17vpw</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Psychedelic, and Intergalactic Princess, sets. </t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uz16sj12lstc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1c17tlk</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Mushies 🍄</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1ggbodfkstc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1c17ee1</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fruit nails!! inspired by pinterest post </t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/om4n65sufstc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1c15qen</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>I love this blue with glitter</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c15qen</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1c14rnk</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>diy ish set???</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c14rnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1c13ec0</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Clear Flower set I did today IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ts8lxxadrtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1c12ysh</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>This hand alone took me three hours 🫣</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hddhmhl9rtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1c12b7m</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>I mixed up a palette &amp; then went wild.</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c12b7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1c11vr0</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Chrome Bugs Bunny🧚🏽</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ni4xhoi0rtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1c10jx4</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Beach themed prom nails</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c10jx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1c0w5e7</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Smiling friends inspired Nail art 🤌🏼✨</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0w5e7</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1c0tynk</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>I love how these pressons blend with the natural nail</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0tynk</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1c0ttfw</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>˚₊‧⁺˖♡˚ I made Kirby nails ˚♡˚₊‧⁺˖ what do you guys think?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0ttfw</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1c0s924</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Mix and Match Nails</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0s924</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1c0oqmz</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Cute mushroom frog nails I did yesterday. I think I'm getting better at nail art :)</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0oqmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1c0mi1j</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>I loved making these flowers shouldn’t have painted them :(</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0mi1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1c0jmma</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Hot Pink Chrome Set. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eq0hj1lc4ntc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1c0jgit</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Graffiti set -part 4</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0jgit</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1c0gt82</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>I’m in love with airbrush 💔</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c0gt82</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Apr 12 08:07:57 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_14.xlsx
+++ b/data/2024_04_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C734"/>
+  <dimension ref="A1:C868"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12911,6 +12911,2284 @@
         </is>
       </c>
     </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1c23arp</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Close up 😍 Aimeili builder base color 156</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c23arp</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1c234rk</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Trying a new BIAB from Amazon 🩷🤍 Love the color</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c234rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1c22gog</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Has anyone ever tried to pinch their natural unpolished nails?</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c22gog/has_anyone_ever_tried_to_pinch_their_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1c22d5v</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Pretty in blue!</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fw7gl742vztc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1c2227j</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2227j</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1c21p2z</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Starburst with aurora rhinestones🌟</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0we7wp9rnztc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1c21a20</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>First time trying to do nail art</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/93o4as07jztc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1c20hzv</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Wedding Nails</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c20hzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1c207wx</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Short chrome nails🥰</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m23y3w528ztc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1c1zy8l</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>New nails (first time doing this 3D shape, be nice)</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1zy8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1c1zxq3</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Tried my best on this set because my fiancée proposed!! 🥳💖</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1zxq3</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1c1ze5g</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Is paraffin wax bad for you?</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c1ze5g/is_paraffin_wax_bad_for_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1c1z4ns</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Will my nails ever go back to normal?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwm3x2pjxytc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1c1yajg</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>New Nails ✨</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1yajg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1c1xsvt</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Base coat for acrylic?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rmmi0ucvlytc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1c1xr3d</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Help for a new Gel x user.</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c1xr3d/help_for_a_new_gel_x_user/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1c1x8ed</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>dashing diva stickers</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9ipzt84hytc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1c1x85b</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Simple &amp; classy 🤍🕊️</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09nzhom2hytc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1c1vb2z</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t xml:space="preserve">guys I need help figuring out how to shape and apply polygel, any tips on how I could improve my form? </t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kqwgs4d91ytc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1c1v9do</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Loved my nails when i got them done but the more i look the more i notice the flaws</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1v9do</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1c1v7ah</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Newbie to nail extensions, what did you think? I’m from Brazil and the translator might be bad</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkl1pu8f0ytc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1c1uyqg</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Efile forward vs reverse </t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c1uyqg/efile_forward_vs_reverse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1c1ut77</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>New nails 💚🖤</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f03u9cdbxxtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1c1undu</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Sweet nails</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pt5hvtu2wxtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1c1ue0u</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>First Gel X</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1ue0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1c1u7j9</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Is this a good nude for me?</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1u7j9</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1c1u3dd</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>What are some decent and affordable gel nail polish brands?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c1u3dd/what_are_some_decent_and_affordable_gel_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1c1sh96</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Gel X Fill?</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c1sh96/gel_x_fill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1c1s9yk</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Wedding nails 💍</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1s9yk</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1c1s5gp</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>New acquisition that I am in love with</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzotfieidxtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1c1rvgr</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Spring French</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgaumbvlbxtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1c1rafs</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>My nails for prom 🤭</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1rafs</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1c1qyfr</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Having a strawberry short cake moment</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15765pj15xtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1c1qu3d</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done Sunday. It’s dip powder and gel. I’m so tired of paying for them to just look like this days later </t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxh7cdw74xtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1c1qsqd</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went with something simple for the first time in a while </t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k842wigy3xtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1c1qdrf</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Show off your mixed shape nail sets🩷</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x10p79j21xtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1c1qdli</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>🐅</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfx3krb11xtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1c1qbw8</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>SpongeBob Nailpants</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1qbw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1c1pu9p</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Nude nails</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1pu9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1c1pqbz</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>It's the cuticle work for me😍</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1pqbz</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1c1pkrk</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Springtime matte sage</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ysc5zsgvwtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1c1pj59</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Cherry blossom birthday nails 🌸</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t9go96l5vwtc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1c1pb0z</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Can I use rubber base gel to build an apex?</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c1pb0z/can_i_use_rubber_base_gel_to_build_an_apex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1c1p6kt</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Sparkle or no sparkle? That is the question…✨💜</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1p6kt</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1c1p030</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Sister and I decided to match nails for coachella this weekend.</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/olnnwzzcrwtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1c1ohd3</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Adding another to the collection! MULTI FACETED 🌅🌅🌅💅</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1ohd3</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1c1o68u</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Had to give my nails a break. </t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vrjvctllwtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1c1o59r</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>should i use rubber base? gel?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzuvaezelwtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1c1nz2c</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I recently got into nail art and this is my first gel x set! I think I did ok. Still a lot to learn! </t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f2ewkhd5kwtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1c1nlde</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t xml:space="preserve">birthday nail set </t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o7zkzktfhwtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1c1ngrw</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>New and back to the almond shape 😌 [f28]. Natural nails with Dip</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ewda5qigwtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1c1n82i</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>✨ ILNP Fairy Dust ✨</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1n82i</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1c1m390</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Need help choosing rhinestones or not</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1m390</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1c1lsgb</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>DND dupe for OPI Put It in Neutral?</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c1lsgb/dnd_dupe_for_opi_put_it_in_neutral/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1c1ld7s</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Black nails!! 🖤⚫️</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxwm8qkj1wtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1c1ky4v</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Lisa Frank-lite</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1ky4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1c1kkgt</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Love me a classic nude pink 😊💕</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owgyi43kvvtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1c1k4bp</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Lava Lamp Vibes ✨</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pqt4df28svtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1c1jm7p</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Reflective Glitter ✨️</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/icif7o9govtc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1c1j9zo</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Advice for press on nails</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1j9zo</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1c1ilpo</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Slug set I did, too weird?</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1ilpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1c1ii7q</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder Gel recommendations </t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c1ii7q/builder_gel_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1c1ih3s</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>My friend got her nails done and painted blueish gray (the color you see) at a salon and then she came to me for the designs. I love how they came out!!</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1ih3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1c1hop6</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>In love with this color!</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwic8v9iavtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1c1ge77</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>1 week nail growth</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pz0hgvf21vtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1c17qax</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Did these nails on myself for a vacation</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c17qax</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1c16idr</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>How do I prevent my natural nails from developing a hook while using builder gel?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c16idr/how_do_i_prevent_my_natural_nails_from_developing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1c1gqn0</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Did my own nails for prom. :)</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6wl8mdm3vtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1c1gl0o</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Mermaid Barbie 🧜🏽‍♀️</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1gl0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1c1fj2r</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Easiest nail system to apply for someone with hand issues on one hand?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c1fj2r/easiest_nail_system_to_apply_for_someone_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1c1fdqe</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Pastel with a little daisy</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3e64sv6ftutc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1c1f8hz</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Water set season 🐬💧🌊</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8bhy9a49sutc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1c1eya0</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>So I guess it’s gel x next!</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c1eya0/so_i_guess_its_gel_x_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1c1epyz</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cruise nails </t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7a2mp7y6outc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1c1e6s8</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Did my nails to look like grandma’s china</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15krb72qjutc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1c1dyej</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Swarovski and Caviar</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1dyej</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1c1bqnl</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>In regards to my last post…</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1bqnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1c1a4xx</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Nude peach with gold tones</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/od2be41ubttc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1c229p7</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Anyone know of a dupe for this green?</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22tkgi2utztc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1c200lr</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Hand painted some lines on my friend</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bs2dz6q26ztc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1c1yod2</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>asking for “polish only” manicure?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c1yod2/asking_for_polish_only_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1c1vec2</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Holo Taco (I’m over brew) 💿✨</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1vec2</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1c1x8u6</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>LL Swamp Girl</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2c4i0ee7hytc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1c1wy5v</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Fiancé is so supportive of my hobby</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1wy5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1c1wvlh</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Finally figured this whole press on fiasco out !</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1wvlh</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1c1wj6a</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>To make up for the snot post</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2cmx297bytc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1c1v0ii</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>M27, I've never painted my nails before but many people say I should, what can be painted in such a short space?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q06xu99uyxtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1c1tylf</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Parrot Polish - Pit Viper Yellow = highlighter yellow</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bfutvwnqqxtc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1c1tfzs</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Siren Call</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1tfzs</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1c1t4xo</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do you guys use to dehydrate your nails?! </t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c1t4xo/what_do_you_guys_use_to_dehydrate_your_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1c1qcd2</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>New to gel, tried a bright french tip.</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzeujhur0xtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1c1pxut</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>LynBDesigns-Aeromancy</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1pxut</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1c1povx</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Mooncat - Snakecharmer</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1povx</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1c1p0tb</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Gotta love that work bathroom light. 💫</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qj4d411mrwtc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1c1nny5</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Sparkly cobalt blue! 💙</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jdt4n962hwtc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1c1niw1</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">When will all of the "coming soon" polishes from LynB be available? </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c1niw1/when_will_all_of_the_coming_soon_polishes_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1c1n8wj</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>✨ ILNP Fairy Dust ✨</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1n8wj</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1c1n7c4</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>✨️🌈Rainbow Gradient🌈✨️</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1n7c4</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1c1mdig</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Spring chrome nails</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1mdig</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1c1m1q5</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>My first dip manicure for fills, with polish on top! Love these colors</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1m1q5</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1c1lsqp</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Spring green🌿🌱</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1lsqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1c1lq19</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Dos, Dont's, Hacks for thickened Peel Off Base (my learnings)</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c1lq19/dos_donts_hacks_for_thickened_peel_off_base_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1c1lpq9</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Former gel user switching to regular polish...recommendations for quick dry drops/top coats?</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c1lpq9/former_gel_user_switching_to_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1c1l6jg</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>I meticulously chose 10 new ILNP polishes to celebrate the new Taylor Swift album release!</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czi1wkxzzvtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1c1js6a</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>i wanna watch wisteria grow right over my bare feet ✨🪻💜</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1js6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1c1jr6c</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>What can I do to make my nails look nicer?</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcfao1sipvtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1c1jqrx</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Great Lakes Lacquer "I'm Well Off My Knees"</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1jqrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1c1jjvr</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Neon Swamp Puppy</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1jjvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1c1ip91</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Do the Mermaid</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1ip91</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1c1ihrx</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Clever Girl on a cloudy day</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1ihrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1c1hvks</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Question about organizing swatches by color</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1hvks</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1c1h7l3</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Lynbdesigns-Your mind is a stream of colors</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1h7l3</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1c1gst5</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Mooncat Head in the Clouds in different lighting</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1gst5</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1c1gssl</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Bright Spring Skittle</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3j3wy8s24vtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1c1fv0i</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Cuticle oil</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c1fv0i/cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1c1ezc8</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Looking for a good OPI red</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c1ezc8/looking_for_a_good_opi_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1c1eg6p</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Is it possible to remove the polish from gel X nails without removing the nail itself?</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c1eg6p/is_it_possible_to_remove_the_polish_from_gel_x/</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1c1ef7v</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Dream within a dream spiral</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1ef7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1c1eawv</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>My Eclipse selection</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/840l16vokutc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1c1e0xs</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>First time trying mooncat</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h63dd43biutc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1c1br55</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>An update on the bottles I couldn't open</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5s27463mvttc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1c1afq0</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Essie Effects, pleasantly surprised</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zu9emypjfttc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1c1adu6</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Bright reds that don't lean pink or coral?</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c1adu6/bright_reds_that_dont_lean_pink_or_coral/</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1c21514</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Starbursts with aurora rhinestones🌟</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ldvm3h5mhztc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1c1ur4u</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Ghostface with French tips 👻❤️</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gi11fiwwxtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1c1rels</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>myscene.com nails</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1rels</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1c1r5yc</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Black &amp; White Set IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x93dm36m6xtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1c1qc4l</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Roarrr</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6rmbpqq0xtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1c1o3yg</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>painted my boyfriends nails for Coachella</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1o3yg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1c1knir</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 🐸 🍄 </t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyjazdu6wvtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1c1hnh0</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Silver or Rose Gold? IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ff6o7bv8avtc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1c1gqfg</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>White plus chrome nails</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1gqfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1c1dwqn</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Caviar and Swarovski</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1dwqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1c1btjc</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A gilded butterfly 🦋 </t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jxzy2kdwttc1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Apr 13 08:03:11 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_14.xlsx
+++ b/data/2024_04_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C868"/>
+  <dimension ref="A1:C1014"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15189,6 +15189,2488 @@
         </is>
       </c>
     </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1c2wmg6</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Why my nails look white or blue?</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1cfn6mmrc7uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1c2wfam</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Hunter X Hunter nails I painted because I’m rewatching the show 🩵</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2wfam</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1c2w7vp</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Spring nails : it is named "Like a princess" 👸💖</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2w7vp</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1c2w12p</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Korean blush nails</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2w12p</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1c2vo4c</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>My 3 week change up</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mvp9ine17uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1c2v12t</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>which color looks the best/natural?</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4g1kc429u6uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1c2uqpp</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Help!!</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mvg0s141r6uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1c2u25l</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Love!!</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bdibxfedj6uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1c2u189</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Bio gel nails keep breaking</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2u189</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1c2tvb0</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4s5ch9eh6uc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1c2tpu9</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>3 months of growth!</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2tpu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1c2swej</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Yay or nay? ❣️</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qkxqcgg776uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1c2solg</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Ceramic inspired</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2solg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1c2rj11</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Some color</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2rj11</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1c2odsz</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Hey, can anyone tell me what nail shape would fit a friend?</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2odsz</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1c2mzwa</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Which photo looks better, 1 or 2? I can't decide.</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2mzwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1c2n2vx</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Gem Patterns</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2n2vx</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1c2t552</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Spring nails</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gtlz47l96uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1c2suw0</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Gel or acrylic nail tips with sticky tabs?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c2suw0/gel_or_acrylic_nail_tips_with_sticky_tabs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1c2refm</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Can I get a gel manicure over a halfway broken nail?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c2refm/can_i_get_a_gel_manicure_over_a_halfway_broken/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1c2r87a</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>ravenclaw vibes💙</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4yhkz67zq5uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1c2r7lr</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>SOS I think I’m getting engaged tomorrow and my nails look awful!</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2r7lr</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1c2r2dr</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Left my dark side and joined the spring. Love or nah?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2r2dr</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1c2qsie</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>nail transformation :)</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2qsie</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1c2qmyp</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>These were so fun to paint!</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2qmyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1c2qj5i</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>So happy with how these turned out ⚫️⚪️⚫️⚪️</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ibin2ngk5uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1c2p1n3</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Could anyone recommend nail supply stores in NYC?</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c2p1n3/could_anyone_recommend_nail_supply_stores_in_nyc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1c2owdd</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Spring gradient nails</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tm20cmer55uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1c2oeo4</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>As promised!! New set!!</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfogr10l15uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1c2nevt</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>I asked for skinny coffins.. did they do me dirty? They're thick and lumpy :(</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2nevt</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1c2n2gh</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time gel extensions </t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c2n2gh/first_time_gel_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1c2ms9c</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you like? It’s deep pink bf chose this color </t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mknsvp6ho4uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1c2mfu7</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Help me strengthen my nails 😭</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2mfu7</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1c2lwyu</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>friday chrome mani ✨ what do you think?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1d0n0ueph4uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1c2lv0r</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>I 🩵 Fridays!</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08ndmd4ah4uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1c2lnu8</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Hand sculpted 3d aliens in care bear customes🩵💚🩷</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2lnu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1c2ljtz</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>New color for me</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2ljtz</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1c2lhvi</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Pressure from somewhere makes the same nail crack the same way. Where could it be coming from?</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2lhvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1c2ld8g</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>cherries!🍒🍒❤️</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2ld8g</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1c2kzn4</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>one more natural mani till crazy birthday nails😁 on me by me</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m73046bpa4uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1c2kr9k</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Been a while since I’ve done my nails!</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2kr9k</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1c2kc09</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Finally got my nails done</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/waek443t54uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1c2jira</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Acrylic set for spring🌸</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2jira</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1c2j1j1</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Yay or nay?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2j1j1</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1c2idsz</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Need color recommendation please! Nude pink dip…</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c2idsz/need_color_recommendation_please_nude_pink_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1c2i5qp</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>4 hours later and I got something amazing</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2i5qp</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1c2i0qn</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>what color nails would look best with this dress?</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4yx1j40no3uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1c2hx28</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Graffiti set - part 5</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2hx28</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1c2hwkr</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>💚</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2hwkr</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1c2hvyz</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Are my nails as terrible as I think?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2hvyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1c2him1</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Would you say my nails grow quickly ?</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2him1</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1c2hcps</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>new set!</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2hcps</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1c2h9sq</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail tech absolutely killed it </t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lclk0pv8j3uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1c2gpeh</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>New to Nails</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c2gpeh/new_to_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1c2gk5o</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Many hours later</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2gk5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1c2g8mp</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Black French stiletto w a twist</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80n7f5qlb3uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1c2fw21</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Am I crazy for wanting this space/gap at my cuticles fixed?</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2fw21</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1c2fpax</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>A fresh lil spring set!</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2fpax</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1c2f7ts</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>My nails doesn't grow equally</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c2f7ts/my_nails_doesnt_grow_equally/</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1c2ey5a</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>What's peeling?</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f5skb9j823uc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1c2exq4</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Long wearing Press ons for Vacation </t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c2exq4/long_wearing_press_ons_for_vacation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1c2evgg</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Kb shimmer? Yuck</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibjgezzo13uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1c2euiq</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need Gel Polish Advice! </t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c2euiq/need_gel_polish_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1c2es9u</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Pink and orange went together well 🥰</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2es9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1c2bgx9</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Hello! How much for this set? Inspo: nailbayo</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pcm2g7g9d2uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1c2eilj</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Lamp that works with beetles gel polish?</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c2eilj/lamp_that_works_with_beetles_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1c2eezv</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Second set I did myself!</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2eezv</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1c2dnp3</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Spring nails 🌼</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7igguwws2uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1c2dixo</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Sparkles all the way. ✨</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2dixo</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1c2coot</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Do these look wonky lol</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r4dqlg2zl2uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1c2ckuh</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>long nails are beautiful ☺️</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbehsyt6l2uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1c2cd5i</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Birthday month nails 💜 I love my nail tech….</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lae3mzkj2uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1c2c6ky</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Left 🤍 and Right ❤️</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/54shth5bi2uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1c2bu5y</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Peeling Nail from Trauma</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c2bu5y/peeling_nail_from_trauma/</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1c2amck</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Spent 7 hours on this. I need to get a life🥲</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2amck</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1c2a0yr</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>You like my nails, what do you think?❤️</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rorlagli22uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1c29333</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>glitterbells hema-free range</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c29333</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1c28s8j</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Love my nail tech 😍</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/056oy3lss1uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1c28fmy</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Nail/skin softening items (in Australia)</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c28fmy/nailskin_softening_items_in_australia/</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1c24atv</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Tacky or fun I cannot decide</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c24atv</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1c20o03</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>I'm getting married soon and trialing these nails, what are your thoughts?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nwawlw1lcztc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1c1zy9x</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>First time using gel/UV lamp, any advice for future attempts?</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1zy9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1c1yy8p</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Question about acrylics/terminology in general?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c1yy8p/question_about_acrylicsterminology_in_general/</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1c1r2n4</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>help?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c1r2n4</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1c27bnu</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Peel off base coat recommendation for natural nail polish, not gel?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c27bnu/peel_off_base_coat_recommendation_for_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1c1jksj</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kinky soft set for spring </t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/73sd4ph6ovtc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1c27fqb</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>nail art attempt #2, lines r getting slightly cleaner, cuticle work is not</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c27fqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1c26s3z</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Get out me swamp!</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32e2pyjpa1uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1c26los</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>First time using/doing soft tip nails and the colours have triggered a millennial core memory but not clearly. (with and without blitz)</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c26los</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1c26h02</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Death Valley Nails - Cochineal</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c26h02</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1c259yy</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Is the apex okay?</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gere83ciu0uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1c24jbu</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>🥰</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1d8dpk5fl0uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1c24fyv</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c24fyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1c2ws3t</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Holo Taco in Europe?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c2ws3t/holo_taco_in_europe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1c2up2r</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>~Aesthetic~ Cruelty Free Brands?</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c2up2r/aesthetic_cruelty_free_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1c2rn1d</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Spring Nails! 💜</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zx03ep6xu5uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1c2rmdu</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Dark nail polish?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c2rmdu/dark_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1c2r02d</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>From the new Death Valley Nails spring collection - But Do Aliens Believe in Me?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2r02d</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1c2qpw1</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>I thought it'd be a love</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2qpw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1c2p1xw</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It's always a great day when your nails and outfit match! </t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vxrnww8175uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1c2opl8</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>The perfect holo match for my skin 😍💿</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ttyv8w445uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1c2oczh</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>First time with londontown town ridge filler basecoat</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2oczh</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1c2nbxp</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Which indie brands have websites that are always open?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c2nbxp/which_indie_brands_have_websites_that_are_always/</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1c2mlrl</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Dupe for Essie Allure or Adore-a-ball</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c2mlrl/dupe_for_essie_allure_or_adoreaball/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1c2lqrc</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>First time outside my comfort zone</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2lqrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1c2kdut</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>What’s your favorite orange?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c2kdut/whats_your_favorite_orange/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1c2k76l</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>pop-a-razzi’s pretty in pearls topper makes such an easy faux- chrome!</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9m3evi8t44uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1c2k3c8</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Distraction mani</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vhzo68y044uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1c2idk7</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Mint chocolate chip mani goodness🍦💅</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5nyr266ar3uc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1c2idk1</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>When does the clock start for thermals?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c2idk1/when_does_the_clock_start_for_thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1c2ibnc</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Lavender Nails using Canmake “Cloudless Sky (82)” with DIY hand ground floral topper (glitter unique suspension base)</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2ibnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1c2hyx5</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Does anyone know why Kelli Marissa stopped reviewing Cirque Colors?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c2hyx5/does_anyone_know_why_kelli_marissa_stopped/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1c2hp5y</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Blue Valentine jelly</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2hp5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1c2hm8a</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Can anyone tell me what style of nails these are? Glitter infused almost? I haven’t been able to find any similar 💔</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hmmtoh5rl3uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1c2gw8o</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Checking cats liking of nails</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2gw8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1c2gs6l</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Great reccomendation!</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2gs6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1c2fqvp</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Always layering Fairy Dust 🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iak96g5483uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1c2f3cr</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Bio seaweed gel</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c2f3cr/bio_seaweed_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1c2dxam</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>ILNP Open Skies</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2dxam</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1c2dxa9</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Cirque Mood Ring + wear update</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2dxa9</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1c2d4ih</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>🌊✨Siren's Songs nail art (PR)</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2d4ih</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1c2cs2w</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>inspired by *spring*</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hwb6bdtnm2uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1c2cfui</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>An ex of mine used to paint my nails, and I always loved how it, and she, made me feel and look. I'm taking back some of that feeling today.</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2cfui</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1c2c6v8</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>🔥💜XMen: Gambit🩷♠️</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2c6v8</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1c2c6kr</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Favorite slept on brands?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2c6kr</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1c2bwg9</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>friday night 🩷</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2bwg9</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1c2antm</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Reflection Pool 🌊</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2antm</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1c28ac8</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>cirque brush replacement?</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c28ac8/cirque_brush_replacement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1c27mt6</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Old Romance</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c27mt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1c26u3w</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Rainy day bad mood mani</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c26u3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1c26ps3</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Get out me swamp!</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/50nk5rw0a1uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1c26igd</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Death Valley Nails - Cochineal</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c26igd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1c26bz3</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Felt like i needed some glitter and pink in my life today</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8xurax761uc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1c2szu4</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>3d water lily</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2szu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1c2qhaf</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>I might have a new passion 👀</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2qhaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1c2p3vg</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painted this giveaway press on set of chandelure 💕 </t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6o9z4r8h75uc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1c2nedr</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Gold 3D Chrome Set. What y’all Think? IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7y8p88qet4uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1c2loz1</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Hand sculpted 3D Alien in care bear customes🩷💚🩵</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2loz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1c2lj9b</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Forgot to post this earlier but yeah… any ideas for my next design? Please recommend anything.😊</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hs5pppuse4uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1c2kuf9</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>7 hours of work. Need to get a life Fr</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2kuf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1c2k2vf</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>my first jujutsu kaisen's nails desing</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2k2vf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1c2j1vz</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>These were my first time, trying hibiscus flowers and not going to lie it kind of made me sad</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2j1vz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1c2hvwa</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Graffiti set -part 5</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2hvwa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1c2d5lc</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Groovy lava lamp nails!</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2d5lc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1c2d0i4</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Art is beautiful </t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ewls0wr9o2uc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1c27452</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Black &amp; White. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xpb3vczd1uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Apr 14 08:18:08 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_04_14.xlsx
+++ b/data/2024_04_14.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1014"/>
+  <dimension ref="A1:C1145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17671,6 +17671,2233 @@
         </is>
       </c>
     </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1c3ogj1</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice </t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c3ogj1/advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1c3objp</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>any tip to get curry stain out of nails quick?</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rg8phyzkjeuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1c3o3fx</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Not only do I buy souvenirs while travelling, I’ll try to do my nails abroad for fun 😄 Around 20€ cat eye nails done in China 💅</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ri61ujtvgeuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1c3nbm8</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>can’t you tell i love swirls 🙈</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3nbm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1c3modh</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>What do you think about guys wearing nail polish?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8unszfg0euc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1c3lxlt</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Current set</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rjl9o42sduc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1c3lc6j</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel Coat on top of press ons </t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c3lc6j/gel_coat_on_top_of_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1c3kp64</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>This is simple but feels fun!</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5r1lp0ymeduc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1c3klqo</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Acrylic girlie trying press ons for the first time! I actually love it. They’re so even 😍 from Salon Perfect at Target</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dxds2tmdduc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1c3kaqt</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Acceleration Prose</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3kaqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1c3ijf7</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Hi assigned male at birth NB here...</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c3ijf7/hi_assigned_male_at_birth_nb_here/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1c3ian0</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Nails of the Week!</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3ian0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1c3k7hg</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Black butler nail design ✨</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k6aeggqd9duc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1c3fpry</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Purple Spring</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3fpry</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1c3fcki</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>X-men inspired nails</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uny6r7cvzbuc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1c3jwdc</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shellac lamp </t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c3jwdc/shellac_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1c3i4oq</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>New nails today 🤍</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3i4oq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1c3h1st</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>eeeee new set</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3h1st</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1c3ghlt</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Please help a mama out.</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c3ghlt/please_help_a_mama_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1c3ghdz</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>what's everyone's thoughts?</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1az77ve9cuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1c3gbvh</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Can I save it?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3gbvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1c3g83s</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Im not sure if i change it bc I feel its not tipy of my color, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tu2mm887cuc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1c3g308</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>They were about to close</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/erianvlz5cuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1c3fbr8</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>do nail salons require a minimum length of natural nails to do acrylics/dip?</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c3fbr8/do_nail_salons_require_a_minimum_length_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1c3f3z8</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Scared of asking for a design </t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c3f3z8/scared_of_asking_for_a_design/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1c3ev2t</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Moody but fun to match the weather lately lol🌦️</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3ev2t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1c3e5t8</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>I like it but feel like they're missing something</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c3e5t8/i_like_it_but_feel_like_theyre_missing_something/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1c3e2co</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Florescent orange coffin🧡</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h16pdqfgpbuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1c3dzkx</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>The skin around my nails grows around and above my nail leaving these lines when they grow out, is filling the sides of my nails the only solution here?</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3dzkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1c3dfz5</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Nails 💅 Yey or Ney ??</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vy0s4g5gkbuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1c3cyp0</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Recovering nail biter. Can't remember the last time I had my nails grown like this. Is the current length okay? What is an appropriate length or how much white should be visible?</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3cyp0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1c3cqgl</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3cqgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1c3ckoy</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Summer Nails</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efubbtbkdbuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1c3cfjf</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Minimalist textures 🐚</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3cfjf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1c394b9</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>I have to wear my nails natural… But they are splitting</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86rlse2imauc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1c3c5oz</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Gel-X Tips for wide nails</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c3c5oz/gelx_tips_for_wide_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1c3c0ae</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Nail Ideas?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c3c0ae/nail_ideas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1c3c02k</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>First time painting stick ons, this is WAY easier than painting my own nails 💀</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3c02k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1c3bqjm</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Wanted 🧡 for April</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xupu35wy6buc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1c3bkqj</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Something simple</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3bkqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1c3birj</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>fresh set ☯️</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vy9ygon85buc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1c3b5s4</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Sprinkle nails! 🧁</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3b5s4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1c3aazi</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Do you like themed manicures?</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0khl60zqvauc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1c3a1ar</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Stop Nails From Peeling Away in Layers?</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a854bt4ntauc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1c39wee</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>What do you think about many nail techs in a salon being unlicensed? Only the manager needs to have a cosmetology license (may differ by state/country)</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c39wee/what_do_you_think_about_many_nail_techs_in_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1c39swq</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Always experimenting with shades of brown and this one suits the best! 🍂</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7avcwhrsrauc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1c39rmt</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>What kind of nail material?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c39rmt/what_kind_of_nail_material/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1c399m6</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Rate my nails</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5p6mnernauc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1c394v4</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Do I need to apply top coat over builder gel before peel base?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c394v4/do_i_need_to_apply_top_coat_over_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1c38zq6</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Is this safe?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c38zq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1c38ryh</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>What are the best types of nails to get for getting engaged?</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c38ryh/what_are_the_best_types_of_nails_to_get_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1c38ntf</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Black again</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlua7wtxiauc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1c37mgh</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Sunglow in the sun’s glow 🌞 (it was a bonus they matched for the Blues game last night)</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i3h6ly7xaauc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1c37db8</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Loving the simplicity</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0i9u2ffx8auc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1c374ei</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>🧜‍♀️💙</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c374ei</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1c37259</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Obsesed with them 😍</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vm66jrmf6auc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1c36q5x</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A Fluid Situation </t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aoo0xayq3auc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1c36kig</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>First successful set of gel x</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c36kig</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1c368q2</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Morning happy Saturday </t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asx1xtsuz9uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1c35twe</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Space Themed Gel Mani</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bhkv8bnhw9uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1c358ue</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>🌟💫✨</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c358ue</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1c34w74</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Frog nails 🥺🐸💚</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c34w74</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1c303x9</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Polygel nails just wotn stick!</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c303x9/polygel_nails_just_wotn_stick/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1c33b5f</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Feels like spring 🌿</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8u61nb3c9uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1c339jo</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Telling nail tech “do whatever you like” 🩷💚🤍</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c339jo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1c32i8t</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails won’t last when doing “clients” </t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c32i8t/nails_wont_last_when_doing_clients/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1c31uiu</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>This pedicure stands as the best I’ve ever had</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0kf7lenz8uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1c31k7j</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Asked my nail tech for pink and fun nails. She nailed it!💕</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fjzbwv93x8uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1c313lx</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Frosted Navy 💙</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/siq01ghws8uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1c312kh</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Glitter watercolor nails</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hl365apms8uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1c30hjk</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Been trying to teach myself how to do nails, how am I doing?</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c30hjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1c2zcci</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>I'm consistently blown away by my nail tech</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/em3zcni4b8uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1c2z7q9</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Shiny Aurora Nails 💫🌌</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2z7q9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1c2yulj</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>subtle shine 💅</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iwokzqx958uc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1c2yqfb</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>spring nails🌈</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7wsggy8w38uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1c2xrqz</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>what polishes could i use to get this kind of look without gel ?</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2xrqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1c2xgbb</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>What is trending this spring?</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1c2xgbb/what_is_trending_this_spring/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1c2wxrx</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>just wanted to post this!</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2wxrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1c2wxkd</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Missed a good red mani🍷</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2wxkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1c2wwpw</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>my nails from the past 2 weeks (natural w/ normal polish)</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2wwpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1c3m892</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Anyone else love matching with their manicure?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3m892</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1c3lxi6</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Pangea is STUNNING</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3lxi6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1c3l975</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pyro 🔥🧨 </t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3dkj93eokduc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1c3kvax</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>This is your reminder that the HHC store is open 👏</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c3kvax/this_is_your_reminder_that_the_hhc_store_is_open/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1c3kkft</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Enchanted Polish</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxeeq1c9dduc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1c3kjey</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Favorite base for French mani?</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c3kjey/favorite_base_for_french_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1c3iv57</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Is a cuticle trim usually extra?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c3iv57/is_a_cuticle_trim_usually_extra/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1c3iwrz</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Fuck. Me. UP.</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3iwrz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1c3gnb9</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best Indie Linears? </t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c3gnb9/best_indie_linears/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1c3gkx8</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>A Human Life is a Beautiful Thing -BKL</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3gkx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1c3gfyd</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>What is the best place to get a wife selection of cheap creams?</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c3gfyd/what_is_the_best_place_to_get_a_wife_selection_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1c3fb4b</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>My new favorite summer mani</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3fb4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1c3emrq</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Blind Man’s Bluff</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/st0n3b12ubuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1c3dkd9</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>had to cut my nails to do a reset😔 asked one of my second graders what i should do for my nails, and she said pink with stars! so, did my own take on it✨</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3dkd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1c3deys</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Dazzle dry pictures/swatches?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c3deys/dazzle_dry_picturesswatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1c3d4ca</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Obsessed is an understatement 😍</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oifzfvgvhbuc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1c3ct3b</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>It's a gas...</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aq44kbjdfbuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1c3c1eq</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>OPI "My Color Wheel is Spinning" 💜</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fymfbi8y8buc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1c3biuz</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Matching the magnolias</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3biuz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1c3awz4</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Londontown base coat ridge filler </t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4yxrlwoi0buc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1c3adxi</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>I am in love &lt;3</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3adxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1c3ac3s</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce - Read Between My Tulips</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3ac3s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1c3a8e3</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>When you want a dark blue extra holo</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3a8e3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1c39uau</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>What's your favorite cuticle balm? I've almost run out of mine 😭</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4qiu6e3sauc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1c395xi</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Emily de Molly Secrets to Keep</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1mbsbd9zmauc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1c38w13</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>I rarely do cremes, but this one is just 🤩</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0q8yu4vkauc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1c38hqh</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Forever obsessed🤠 </t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bvyrhisqhauc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1c37piu</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Barry M, my go to drugstore brand</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c37piu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1c37k4s</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Sunglow in the sun’s glow 🌞 (it was a bonus they matched for the Blues game last night)</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2g92zabdaauc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1c37i6m</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Mani of the week</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c37i6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1c36xj7</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Orly Color Pass issue</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c36xj7/orly_color_pass_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1c359h2</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>🌟💫✨</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c359h2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1c34xjt</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Non-Boring Brown</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xc218xa7p9uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1c34kvc</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Racks that fit China Glaze</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uw1i0xhcm9uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1c32oaz</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Leaf by Example (and some things that look like it)</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c32oaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1c31yx7</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Gel x - partial removal</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1c31yx7/gel_x_partial_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1c30n7z</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Baseball</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qd8ayh7lo8uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1c31972</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Stiff As a Board</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c31972</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1c30i5c</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Wtf man</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c30i5c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1c307np</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Fairy Dust over Queen of the Dead</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u1xjojyek8uc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1c307ob</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They have only ever removed shellac with e-file and regular file in see saw motion. </t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uw2ro3ggk8uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1c2zlyo</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Polished for Days Lush</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c2zlyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1c3oezx</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Creating my own nail foils</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xgjs5nrkeuc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1c3m5eq</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>In love</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5u6ym14huduc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1c38k43</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Flowers and Strawberries Nails for Spring</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c38k43</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1c3727d</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>🧜‍♀️💙</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c3727d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1c32rg0</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Fizzarolli (Helluva Boss) inspired nails!</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c32rg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1c32m9n</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Freestyle set, took 10 hours 🤭 the bunny glows!</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1c32m9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1c32ief</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Updated: my fiancé’s latest design! Hand painted!</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8q50kukf59uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1c31max</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Adventure Time! </t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y7naiv8mx8uc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1c2zoz8</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Ideas?</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mh2xgio0f8uc1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>